<commit_message>
Added template for designer input form.
</commit_message>
<xml_diff>
--- a/reference/AndysBatteryPackFittingTool.xlsx
+++ b/reference/AndysBatteryPackFittingTool.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="207">
   <si>
     <t>X</t>
   </si>
@@ -634,6 +634,12 @@
   </si>
   <si>
     <t>kg</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>name_oem</t>
   </si>
 </sst>
 </file>
@@ -13311,8 +13317,8 @@
   </sheetPr>
   <dimension ref="A4:P42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13493,6 +13499,12 @@
       <c r="L13" t="s">
         <v>108</v>
       </c>
+      <c r="N13" t="s">
+        <v>205</v>
+      </c>
+      <c r="O13" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
@@ -13518,6 +13530,12 @@
       </c>
       <c r="L14" t="s">
         <v>108</v>
+      </c>
+      <c r="N14" t="s">
+        <v>206</v>
+      </c>
+      <c r="O14" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">

</xml_diff>